<commit_message>
update for challenge 27
</commit_message>
<xml_diff>
--- a/26 - StructuredDataValidationBot/input/InputData.xlsx
+++ b/26 - StructuredDataValidationBot/input/InputData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\UiPath\RPAChallengeByRobotICT\26-Structured Data Validation\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dongovor\Documents\UiPath\RPAChallengeByRobotict_full\26.1 - StructuredDataValidationBot\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD60286-02E9-4815-B3BF-631EA5991C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21CAFA6-FA9C-40EF-AA63-FC835CC00FF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="1500" windowWidth="25815" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20940" yWindow="1770" windowWidth="29760" windowHeight="16905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -65,6 +65,9 @@
     <t>2021-09-02</t>
   </si>
   <si>
+    <t>2021-02-29</t>
+  </si>
+  <si>
     <t>2021-02-02</t>
   </si>
   <si>
@@ -257,13 +260,19 @@
     <t>Can only contain "APPROVED" or "REJECTED"</t>
   </si>
   <si>
-    <t>154</t>
-  </si>
-  <si>
-    <t>222</t>
-  </si>
-  <si>
-    <t>2021-02-29</t>
+    <t>Must match one of the Error codes in Sheet ErrorCodes</t>
+  </si>
+  <si>
+    <t>Must match one of the Errror Names in Sheet ErrorCodes</t>
+  </si>
+  <si>
+    <t>Must contain "YES" or "NO"</t>
+  </si>
+  <si>
+    <t>If column "Registered" is "YES", then column "RegisteredBy" must be filled in and vice versa (If column "Registered" is "NO", then column "RegisteredBy" must be filled in)</t>
+  </si>
+  <si>
+    <t>If "Result" = "APPROVED", only column "ApprovedBy" must be filled in, "RejectedBy" must be empty (and vice versa, for "REJECTED")</t>
   </si>
 </sst>
 </file>
@@ -301,7 +310,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -309,17 +318,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -605,7 +624,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,431 +637,417 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2">
+        <v>154</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2">
+        <v>222</v>
+      </c>
+      <c r="D3" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="G12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" s="6" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
         <v>72</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="I13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="C14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="G14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="7" t="s">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="D15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="5" t="s">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="2">
+        <v>879</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="G16" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" s="5" t="s">
+      <c r="I16" t="s">
         <v>69</v>
-      </c>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="3">
-        <v>879</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -1083,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA09503-DD8D-45A2-8CBA-00B68C6958E6}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,15 +1099,15 @@
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1110,10 +1115,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1121,10 +1126,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1132,22 +1137,76 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>75</v>
+      <c r="C5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1178,7 +1237,7 @@
         <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1186,23 +1245,23 @@
         <v>222</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,31 +1269,31 @@
         <v>879</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1242,7 +1301,7 @@
         <v>810</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>